<commit_message>
First Commit on Gandi
</commit_message>
<xml_diff>
--- a/TourDeFrance.xlsx
+++ b/TourDeFrance.xlsx
@@ -941,7 +941,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="E7" sqref="E7:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.140625" defaultRowHeight="15"/>
@@ -1021,7 +1021,7 @@
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -1032,18 +1032,6 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1060,32 +1048,32 @@
       <c r="D7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="E7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1">
       <c r="A8" s="18"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
-      <c r="E8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="E8" s="5"/>
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1094,6 +1082,18 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
+      <c r="E9" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1">
       <c r="A10" s="11" t="s">

</xml_diff>